<commit_message>
further progress on signs
</commit_message>
<xml_diff>
--- a/AnimalDiseaseQueryWebApp/Files/master_list.xlsx
+++ b/AnimalDiseaseQueryWebApp/Files/master_list.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Crawford\Dropbox\2 Research\2017_19 EBTI and Brooke\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spike\source\repos\AnimalDiseaseQueryPage\AnimalDiseaseQueryWebApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B57C334-4D14-4C39-B410-1076CC1F6A18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="72" windowWidth="13116" windowHeight="9996" tabRatio="652" activeTab="2"/>
+    <workbookView xWindow="180" yWindow="75" windowWidth="13110" windowHeight="9990" tabRatio="652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="11" r:id="rId1"/>
@@ -17,17 +18,24 @@
     <sheet name="Diseases" sheetId="14" r:id="rId3"/>
     <sheet name="Sheep vs Goat" sheetId="7" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Crawford</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -52,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -81,12 +89,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Crawford</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -116,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="146">
   <si>
     <t>Constipation</t>
   </si>
@@ -392,9 +400,6 @@
     <t>(A number are in fact combined signs - designed to capture a wider range of clinical presentations while minimising the size of the probability matrix required.)</t>
   </si>
   <si>
-    <t>(In EDDiE)</t>
-  </si>
-  <si>
     <t>Equids</t>
   </si>
   <si>
@@ -641,7 +646,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -911,6 +916,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -946,6 +968,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1121,63 +1160,63 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="13.77734375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="173.77734375" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="173.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>75</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1187,24 +1226,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="65.33203125" style="4" customWidth="1"/>
-    <col min="3" max="6" width="6.6640625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="2.5546875" style="4" customWidth="1"/>
-    <col min="8" max="8" width="70.109375" style="12" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="3.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="65.28515625" style="4" customWidth="1"/>
+    <col min="3" max="6" width="6.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="2.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="70.140625" style="12" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
@@ -1226,7 +1265,7 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
     </row>
-    <row r="2" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1240,7 +1279,7 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
     </row>
-    <row r="3" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>66</v>
       </c>
@@ -1254,7 +1293,7 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
     </row>
-    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>33</v>
       </c>
@@ -1271,9 +1310,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1288,7 +1327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
         <v>67</v>
       </c>
@@ -1297,10 +1336,10 @@
         <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="24" t="s">
         <v>3</v>
       </c>
@@ -1317,7 +1356,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
         <v>68</v>
       </c>
@@ -1326,7 +1365,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>69</v>
       </c>
@@ -1335,7 +1374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
         <v>64</v>
       </c>
@@ -1344,7 +1383,7 @@
       </c>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="13" t="s">
         <v>0</v>
       </c>
@@ -1357,7 +1396,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="13" t="s">
         <v>4</v>
       </c>
@@ -1367,9 +1406,9 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>19</v>
@@ -1379,10 +1418,10 @@
       </c>
       <c r="F13" s="22"/>
       <c r="H13" s="12" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="13" t="s">
         <v>1</v>
       </c>
@@ -1399,7 +1438,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="24" t="s">
         <v>5</v>
       </c>
@@ -1414,7 +1453,7 @@
       </c>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="24" t="s">
         <v>6</v>
       </c>
@@ -1429,7 +1468,7 @@
       </c>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>70</v>
       </c>
@@ -1438,7 +1477,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="24" t="s">
         <v>7</v>
       </c>
@@ -1451,7 +1490,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
         <v>65</v>
       </c>
@@ -1462,7 +1501,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="24" t="s">
         <v>15</v>
       </c>
@@ -1471,7 +1510,7 @@
       </c>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="7" t="s">
         <v>34</v>
       </c>
@@ -1488,7 +1527,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>62</v>
       </c>
@@ -1497,7 +1536,7 @@
       </c>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
         <v>71</v>
       </c>
@@ -1506,7 +1545,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>72</v>
       </c>
@@ -1515,7 +1554,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
         <v>73</v>
       </c>
@@ -1524,7 +1563,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="13" t="s">
         <v>13</v>
       </c>
@@ -1536,7 +1575,7 @@
       </c>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="7" t="s">
         <v>8</v>
       </c>
@@ -1553,7 +1592,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="24" t="s">
         <v>9</v>
       </c>
@@ -1568,7 +1607,7 @@
       </c>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>10</v>
       </c>
@@ -1583,7 +1622,7 @@
       </c>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="24" t="s">
         <v>11</v>
       </c>
@@ -1600,7 +1639,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
@@ -1609,7 +1648,7 @@
       </c>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>2</v>
       </c>
@@ -1626,7 +1665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="24" t="s">
         <v>12</v>
       </c>
@@ -1643,29 +1682,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="22"/>
     </row>
-    <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="23">
-        <f>COUNTIF(C2:C34, "X")</f>
-        <v>15</v>
-      </c>
-      <c r="D35" s="23">
-        <f>COUNTIF(D2:D34, "X")</f>
-        <v>18</v>
-      </c>
-      <c r="E35" s="23">
-        <f>COUNTIF(E2:E34, "X")</f>
-        <v>21</v>
-      </c>
-      <c r="F35" s="23">
-        <f>COUNTIF(F2:F34, "X")</f>
-        <v>18</v>
-      </c>
+    <row r="35" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="8"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
     </row>
   </sheetData>
   <sortState ref="B133:B209">
@@ -1678,29 +1703,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B1:J50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" activePane="bottomLeft"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="570" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1:B1048576"/>
       <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5546875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="28.6640625" style="4" customWidth="1"/>
-    <col min="3" max="5" width="6.6640625" style="5" customWidth="1"/>
-    <col min="6" max="8" width="6.6640625" style="22" customWidth="1"/>
-    <col min="9" max="9" width="2.5546875" style="4" customWidth="1"/>
-    <col min="10" max="10" width="95.88671875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="4.33203125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="21.33203125" style="4" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="3.5703125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="4" customWidth="1"/>
+    <col min="3" max="5" width="6.7109375" style="5" customWidth="1"/>
+    <col min="6" max="8" width="6.7109375" style="22" customWidth="1"/>
+    <col min="9" max="9" width="2.5703125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="95.85546875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="4.28515625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
@@ -1717,26 +1742,26 @@
         <v>24</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>89</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>90</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
         <v>91</v>
-      </c>
-      <c r="G2" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="4" t="s">
-        <v>92</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>19</v>
@@ -1753,9 +1778,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1766,9 +1791,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1782,9 +1807,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>19</v>
@@ -1792,59 +1817,59 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="4" t="s">
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B8" s="4" t="s">
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="4" t="s">
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="F9" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F9" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B10" s="4" t="s">
+      <c r="D10" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B11" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>26</v>
       </c>
@@ -1858,10 +1883,10 @@
         <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
@@ -1875,131 +1900,131 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B15" s="4" t="s">
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="4" t="s">
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B16" s="4" t="s">
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="4" t="s">
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B17" s="4" t="s">
+      <c r="G17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B18" s="4" t="s">
+      <c r="G18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B19" s="4" t="s">
+      <c r="G19" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B20" s="4" t="s">
+      <c r="D20" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B21" s="4" t="s">
+      <c r="G21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="4" t="s">
+      <c r="F22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="F22" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="4" t="s">
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="4" t="s">
+      <c r="D23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="4" t="s">
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>22</v>
       </c>
@@ -2013,26 +2038,26 @@
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="2:10" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="G26" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B27" s="4" t="s">
-        <v>120</v>
-      </c>
       <c r="G27" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
@@ -2052,29 +2077,29 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="4" t="s">
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B30" s="4" t="s">
-        <v>123</v>
-      </c>
       <c r="D30" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>23</v>
       </c>
@@ -2091,29 +2116,29 @@
         <v>19</v>
       </c>
       <c r="J31" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B32" s="4" t="s">
+      <c r="F32" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="F32" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B33" s="4" t="s">
+      <c r="C33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>31</v>
       </c>
@@ -2127,10 +2152,10 @@
         <v>19</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="35" spans="2:10" x14ac:dyDescent="0.3">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
@@ -2141,125 +2166,125 @@
         <v>19</v>
       </c>
       <c r="J35" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="36" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B36" s="4" t="s">
+      <c r="F36" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="F36" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B37" s="4" t="s">
+      <c r="C37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="4" t="s">
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="38" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B38" s="4" t="s">
+      <c r="F38" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F38" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="4" t="s">
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="39" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B39" s="4" t="s">
+      <c r="G39" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G39" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H39" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B40" s="4" t="s">
+      <c r="G40" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H40" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G40" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H40" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B41" s="4" t="s">
+      <c r="G41" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H41" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="G41" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H41" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B42" s="4" t="s">
+      <c r="G42" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H42" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B43" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G42" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H42" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B43" s="6" t="s">
+      <c r="F43" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B44" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="F43" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B44" s="4" t="s">
+      <c r="G44" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B45" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="G44" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B45" s="4" t="s">
+      <c r="G45" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H45" s="22" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B46" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="G45" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B46" s="7" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B47" s="4" t="s">
         <v>30</v>
       </c>
@@ -2273,37 +2298,37 @@
       <c r="G47" s="16"/>
       <c r="H47" s="16"/>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="C48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H48" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="4" t="s">
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B49" s="4" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B49" s="4" t="s">
+      <c r="C49" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B50" s="8" t="s">
         <v>145</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B50" s="8" t="s">
-        <v>146</v>
       </c>
       <c r="C50" s="23">
         <f t="shared" ref="C50:H50" si="0">COUNTIF(C2:C49, "X")</f>
@@ -2338,23 +2363,23 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:V39"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="4" customWidth="1"/>
-    <col min="3" max="14" width="8.6640625" customWidth="1"/>
-    <col min="21" max="21" width="3.6640625" customWidth="1"/>
-    <col min="22" max="22" width="18.5546875" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" style="4" customWidth="1"/>
+    <col min="3" max="14" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="3.7109375" customWidth="1"/>
+    <col min="22" max="22" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
@@ -2419,7 +2444,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
@@ -2481,7 +2506,7 @@
         <v>11.875</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
@@ -2543,7 +2568,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>21</v>
       </c>
@@ -2605,7 +2630,7 @@
         <v>29.375</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
@@ -2667,7 +2692,7 @@
         <v>8.75</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>27</v>
       </c>
@@ -2732,7 +2757,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -2797,7 +2822,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
@@ -2859,7 +2884,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>22</v>
       </c>
@@ -2921,7 +2946,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>28</v>
       </c>
@@ -2983,7 +3008,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>28</v>
       </c>
@@ -3045,7 +3070,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>23</v>
       </c>
@@ -3107,7 +3132,7 @@
         <v>32.5</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>23</v>
       </c>
@@ -3169,7 +3194,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>31</v>
       </c>
@@ -3231,7 +3256,7 @@
         <v>58.75</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
@@ -3293,7 +3318,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>29</v>
       </c>
@@ -3355,7 +3380,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>29</v>
       </c>
@@ -3417,7 +3442,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
@@ -3479,7 +3504,7 @@
         <v>58.75</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>30</v>
       </c>
@@ -3541,7 +3566,7 @@
         <v>76.25</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="14"/>
       <c r="B20" s="5"/>
       <c r="C20" s="15"/>
@@ -3563,7 +3588,7 @@
       <c r="S20" s="15"/>
       <c r="T20" s="15"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>57</v>
       </c>
@@ -3622,7 +3647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
@@ -3702,7 +3727,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>26</v>
       </c>
@@ -3710,7 +3735,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>21</v>
       </c>
@@ -3790,7 +3815,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
@@ -3798,7 +3823,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
@@ -3875,12 +3900,12 @@
         <v>-4.75</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>22</v>
       </c>
@@ -3957,12 +3982,12 @@
         <v>-0.38</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>28</v>
       </c>
@@ -4039,12 +4064,12 @@
         <v>-0.35</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>23</v>
       </c>
@@ -4121,12 +4146,12 @@
         <v>-0.96923076923076923</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>31</v>
       </c>
@@ -4203,12 +4228,12 @@
         <v>0.63194444444444442</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>29</v>
       </c>
@@ -4285,12 +4310,12 @@
         <v>-0.15151515151515152</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
         <v>30</v>
       </c>
@@ -4367,7 +4392,7 @@
         <v>-0.2978723404255319</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
sign core table added
</commit_message>
<xml_diff>
--- a/AnimalDiseaseQueryWebApp/Files/master_list.xlsx
+++ b/AnimalDiseaseQueryWebApp/Files/master_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spike\source\repos\AnimalDiseaseQueryPage\AnimalDiseaseQueryWebApp\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B57C334-4D14-4C39-B410-1076CC1F6A18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D24B775-D182-4FAE-B39B-38FED9D0438E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="180" yWindow="75" windowWidth="13110" windowHeight="9990" tabRatio="652" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,9 +361,6 @@
     <t>Sudden death</t>
   </si>
   <si>
-    <t>Congessed mucous membrane</t>
-  </si>
-  <si>
     <t>Hair loss (alopecia)</t>
   </si>
   <si>
@@ -641,6 +638,9 @@
   </si>
   <si>
     <t>(In App)</t>
+  </si>
+  <si>
+    <t>Congested mm</t>
   </si>
 </sst>
 </file>
@@ -1176,15 +1176,15 @@
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="2:3" x14ac:dyDescent="0.25">
@@ -1192,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="2:3" x14ac:dyDescent="0.25">
@@ -1200,23 +1200,23 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -1229,8 +1229,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:F35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1257,7 +1257,7 @@
         <v>24</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H1" s="11" t="s">
         <v>20</v>
@@ -1281,7 +1281,7 @@
     </row>
     <row r="3" spans="2:10" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1312,7 +1312,7 @@
     </row>
     <row r="5" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1329,14 +1329,14 @@
     </row>
     <row r="6" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="22"/>
       <c r="F6" s="22" t="s">
         <v>19</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1358,7 +1358,7 @@
     </row>
     <row r="8" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E8" s="22"/>
       <c r="F8" s="5" t="s">
@@ -1367,7 +1367,7 @@
     </row>
     <row r="9" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E9" s="22"/>
       <c r="F9" s="5" t="s">
@@ -1376,7 +1376,7 @@
     </row>
     <row r="10" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="25" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>19</v>
@@ -1408,7 +1408,7 @@
     </row>
     <row r="13" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>19</v>
@@ -1418,7 +1418,7 @@
       </c>
       <c r="F13" s="22"/>
       <c r="H13" s="12" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1470,7 +1470,7 @@
     </row>
     <row r="17" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E17" s="22"/>
       <c r="F17" s="22" t="s">
@@ -1492,7 +1492,7 @@
     </row>
     <row r="19" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="22" t="s">
         <v>19</v>
@@ -1538,7 +1538,7 @@
     </row>
     <row r="23" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E23" s="22"/>
       <c r="F23" s="22" t="s">
@@ -1547,7 +1547,7 @@
     </row>
     <row r="24" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="22" t="s">
@@ -1556,7 +1556,7 @@
     </row>
     <row r="25" spans="2:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E25" s="22"/>
       <c r="F25" s="22" t="s">
@@ -1742,10 +1742,10 @@
         <v>24</v>
       </c>
       <c r="G1" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="H1" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>89</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>20</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>19</v>
@@ -1761,7 +1761,7 @@
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>19</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
@@ -1793,7 +1793,7 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>19</v>
@@ -1809,7 +1809,7 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>19</v>
@@ -1819,35 +1819,35 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>95</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="4" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>97</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F9" s="22" t="s">
         <v>19</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>19</v>
@@ -1863,7 +1863,7 @@
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>19</v>
@@ -1883,7 +1883,7 @@
         <v>19</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
@@ -1902,37 +1902,37 @@
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J16" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>19</v>
@@ -1943,7 +1943,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>19</v>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>19</v>
@@ -1965,18 +1965,18 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>19</v>
@@ -1987,41 +1987,41 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="F22" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="F22" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J23" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F23" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>19</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
@@ -2038,12 +2038,12 @@
         <v>19</v>
       </c>
       <c r="J25" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B26" s="26" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G26" s="22" t="s">
         <v>19</v>
@@ -2051,7 +2051,7 @@
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G27" s="22" t="s">
         <v>19</v>
@@ -2079,21 +2079,21 @@
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>19</v>
@@ -2116,12 +2116,12 @@
         <v>19</v>
       </c>
       <c r="J31" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F32" s="22" t="s">
         <v>19</v>
@@ -2129,13 +2129,13 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C33" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
         <v>19</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.25">
@@ -2166,12 +2166,12 @@
         <v>19</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B36" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F36" s="22" t="s">
         <v>19</v>
@@ -2179,35 +2179,35 @@
     </row>
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H37" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B38" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F38" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" s="4" t="s">
         <v>132</v>
-      </c>
-      <c r="F38" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G39" s="22" t="s">
         <v>19</v>
@@ -2218,7 +2218,7 @@
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B40" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G40" s="22" t="s">
         <v>19</v>
@@ -2229,7 +2229,7 @@
     </row>
     <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B41" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G41" s="22" t="s">
         <v>19</v>
@@ -2240,7 +2240,7 @@
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B42" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G42" s="22" t="s">
         <v>19</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F43" s="22" t="s">
         <v>19</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B44" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G44" s="22" t="s">
         <v>19</v>
@@ -2270,7 +2270,7 @@
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G45" s="22" t="s">
         <v>19</v>
@@ -2281,7 +2281,7 @@
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B46" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.25">
@@ -2300,27 +2300,27 @@
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B48" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H48" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>142</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H48" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>19</v>
@@ -2328,7 +2328,7 @@
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C50" s="23">
         <f t="shared" ref="C50:H50" si="0">COUNTIF(C2:C49, "X")</f>

</xml_diff>